<commit_message>
states up to Ohio
</commit_message>
<xml_diff>
--- a/pixel-measurements.xlsx
+++ b/pixel-measurements.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Arkansas</t>
   </si>
@@ -148,6 +148,18 @@
   </si>
   <si>
     <t>New Hampshire</t>
+  </si>
+  <si>
+    <t>New Jersey</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>North Carolina</t>
+  </si>
+  <si>
+    <t>Ohio</t>
   </si>
 </sst>
 </file>
@@ -196,8 +208,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="85">
+  <cellStyleXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -286,7 +318,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="85">
+  <cellStyles count="105">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -329,6 +361,16 @@
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -371,6 +413,16 @@
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -700,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S24"/>
+  <dimension ref="A1:S28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+      <selection activeCell="Q28" sqref="Q28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -877,7 +929,7 @@
         <v>191</v>
       </c>
       <c r="R3">
-        <f t="shared" ref="R3:R24" si="0">SUM(C3+F3+I3+L3+O3)-AVERAGE(SUM(E3+D3),SUM(G3+H3),SUM(J3+K3), SUM(M3:N3),SUM(P3:Q3))</f>
+        <f t="shared" ref="R3:R28" si="0">SUM(C3+F3+I3+L3+O3)-AVERAGE(SUM(E3+D3),SUM(G3+H3),SUM(J3+K3), SUM(M3:N3),SUM(P3:Q3))</f>
         <v>-3</v>
       </c>
     </row>
@@ -2087,6 +2139,251 @@
       <c r="R24">
         <f t="shared" si="0"/>
         <v>-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19">
+      <c r="A25" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25">
+        <v>46</v>
+      </c>
+      <c r="C25">
+        <v>64</v>
+      </c>
+      <c r="D25">
+        <v>445</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>98</v>
+      </c>
+      <c r="G25">
+        <v>378</v>
+      </c>
+      <c r="H25">
+        <f>445-G25</f>
+        <v>67</v>
+      </c>
+      <c r="I25">
+        <v>49</v>
+      </c>
+      <c r="J25">
+        <v>434</v>
+      </c>
+      <c r="K25">
+        <f>445-J25</f>
+        <v>11</v>
+      </c>
+      <c r="L25">
+        <v>81</v>
+      </c>
+      <c r="M25">
+        <v>289</v>
+      </c>
+      <c r="N25">
+        <f>445-M25</f>
+        <v>156</v>
+      </c>
+      <c r="O25">
+        <v>152</v>
+      </c>
+      <c r="P25">
+        <v>222</v>
+      </c>
+      <c r="Q25">
+        <f>445-P25</f>
+        <v>223</v>
+      </c>
+      <c r="R25">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19">
+      <c r="A26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26">
+        <v>45</v>
+      </c>
+      <c r="C26">
+        <v>74</v>
+      </c>
+      <c r="D26">
+        <v>451</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>91</v>
+      </c>
+      <c r="G26">
+        <v>371</v>
+      </c>
+      <c r="H26">
+        <f>451-G26</f>
+        <v>80</v>
+      </c>
+      <c r="I26">
+        <v>45</v>
+      </c>
+      <c r="J26">
+        <v>439</v>
+      </c>
+      <c r="K26">
+        <f>451-J26</f>
+        <v>12</v>
+      </c>
+      <c r="L26">
+        <v>79</v>
+      </c>
+      <c r="M26">
+        <v>255</v>
+      </c>
+      <c r="N26">
+        <f>451-M26</f>
+        <v>196</v>
+      </c>
+      <c r="O26">
+        <v>159</v>
+      </c>
+      <c r="P26">
+        <v>230</v>
+      </c>
+      <c r="Q26">
+        <f>451-P26</f>
+        <v>221</v>
+      </c>
+      <c r="R26">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19">
+      <c r="A27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27">
+        <v>71</v>
+      </c>
+      <c r="C27">
+        <v>255</v>
+      </c>
+      <c r="D27">
+        <v>352</v>
+      </c>
+      <c r="E27">
+        <f>403-D27</f>
+        <v>51</v>
+      </c>
+      <c r="F27">
+        <v>22</v>
+      </c>
+      <c r="G27">
+        <v>349</v>
+      </c>
+      <c r="H27">
+        <f>403-G27</f>
+        <v>54</v>
+      </c>
+      <c r="I27">
+        <v>10</v>
+      </c>
+      <c r="J27">
+        <v>397</v>
+      </c>
+      <c r="K27">
+        <f>403-J27</f>
+        <v>6</v>
+      </c>
+      <c r="L27">
+        <v>50</v>
+      </c>
+      <c r="M27">
+        <v>179</v>
+      </c>
+      <c r="N27">
+        <f>403-M27</f>
+        <v>224</v>
+      </c>
+      <c r="O27">
+        <v>59</v>
+      </c>
+      <c r="P27">
+        <v>206</v>
+      </c>
+      <c r="Q27">
+        <f>403-P27</f>
+        <v>197</v>
+      </c>
+      <c r="R27">
+        <f t="shared" si="0"/>
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19">
+      <c r="A28" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28">
+        <v>33</v>
+      </c>
+      <c r="C28">
+        <v>127</v>
+      </c>
+      <c r="D28">
+        <v>473</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>62</v>
+      </c>
+      <c r="G28">
+        <v>421</v>
+      </c>
+      <c r="H28">
+        <f>473-G28</f>
+        <v>52</v>
+      </c>
+      <c r="I28">
+        <v>27</v>
+      </c>
+      <c r="J28">
+        <v>466</v>
+      </c>
+      <c r="K28">
+        <f>473-J28</f>
+        <v>7</v>
+      </c>
+      <c r="L28">
+        <v>53</v>
+      </c>
+      <c r="M28">
+        <v>290</v>
+      </c>
+      <c r="N28">
+        <f>473-M28</f>
+        <v>183</v>
+      </c>
+      <c r="O28">
+        <v>201</v>
+      </c>
+      <c r="P28">
+        <v>240</v>
+      </c>
+      <c r="Q28">
+        <f>473-P28</f>
+        <v>233</v>
+      </c>
+      <c r="R28">
+        <f t="shared" si="0"/>
+        <v>-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
up to Rhode Island
</commit_message>
<xml_diff>
--- a/pixel-measurements.xlsx
+++ b/pixel-measurements.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Arkansas</t>
   </si>
@@ -160,6 +160,15 @@
   </si>
   <si>
     <t>Ohio</t>
+  </si>
+  <si>
+    <t>Oregon</t>
+  </si>
+  <si>
+    <t>Pennsylvania</t>
+  </si>
+  <si>
+    <t>Rhode Island</t>
   </si>
 </sst>
 </file>
@@ -208,8 +217,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="105">
+  <cellStyleXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -318,7 +341,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="105">
+  <cellStyles count="119">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -371,6 +394,13 @@
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -423,6 +453,13 @@
     <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -752,10 +789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S28"/>
+  <dimension ref="A1:S31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q28" sqref="Q28"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -929,7 +966,7 @@
         <v>191</v>
       </c>
       <c r="R3">
-        <f t="shared" ref="R3:R28" si="0">SUM(C3+F3+I3+L3+O3)-AVERAGE(SUM(E3+D3),SUM(G3+H3),SUM(J3+K3), SUM(M3:N3),SUM(P3:Q3))</f>
+        <f t="shared" ref="R3:R31" si="0">SUM(C3+F3+I3+L3+O3)-AVERAGE(SUM(E3+D3),SUM(G3+H3),SUM(J3+K3), SUM(M3:N3),SUM(P3:Q3))</f>
         <v>-3</v>
       </c>
     </row>
@@ -2384,6 +2421,189 @@
       <c r="R28">
         <f t="shared" si="0"/>
         <v>-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19">
+      <c r="A29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29">
+        <v>38</v>
+      </c>
+      <c r="C29">
+        <v>125</v>
+      </c>
+      <c r="D29">
+        <v>468</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>85</v>
+      </c>
+      <c r="G29">
+        <v>463</v>
+      </c>
+      <c r="H29">
+        <f>D29-G29</f>
+        <v>5</v>
+      </c>
+      <c r="I29">
+        <v>24</v>
+      </c>
+      <c r="J29">
+        <v>468</v>
+      </c>
+      <c r="K29">
+        <f>468-J29</f>
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>59</v>
+      </c>
+      <c r="M29">
+        <v>419</v>
+      </c>
+      <c r="N29">
+        <f>468-M29</f>
+        <v>49</v>
+      </c>
+      <c r="O29">
+        <v>168</v>
+      </c>
+      <c r="P29">
+        <v>244</v>
+      </c>
+      <c r="Q29">
+        <f>468-P29</f>
+        <v>224</v>
+      </c>
+      <c r="R29">
+        <f t="shared" si="0"/>
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19">
+      <c r="A30" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30">
+        <v>50</v>
+      </c>
+      <c r="C30">
+        <v>67</v>
+      </c>
+      <c r="D30">
+        <v>442</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>89</v>
+      </c>
+      <c r="G30">
+        <v>392</v>
+      </c>
+      <c r="H30">
+        <f>442-G30</f>
+        <v>50</v>
+      </c>
+      <c r="I30">
+        <v>33</v>
+      </c>
+      <c r="J30">
+        <v>425</v>
+      </c>
+      <c r="K30">
+        <f>442-J30</f>
+        <v>17</v>
+      </c>
+      <c r="L30">
+        <v>70</v>
+      </c>
+      <c r="M30">
+        <v>300</v>
+      </c>
+      <c r="N30">
+        <f>442-M30</f>
+        <v>142</v>
+      </c>
+      <c r="O30">
+        <v>181</v>
+      </c>
+      <c r="P30">
+        <v>222</v>
+      </c>
+      <c r="Q30">
+        <f>442-P30</f>
+        <v>220</v>
+      </c>
+      <c r="R30">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19">
+      <c r="A31" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31">
+        <v>42</v>
+      </c>
+      <c r="C31">
+        <v>46</v>
+      </c>
+      <c r="D31">
+        <v>455</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>176</v>
+      </c>
+      <c r="G31">
+        <v>316</v>
+      </c>
+      <c r="H31">
+        <f>455-G31</f>
+        <v>139</v>
+      </c>
+      <c r="I31">
+        <v>33</v>
+      </c>
+      <c r="J31">
+        <v>444</v>
+      </c>
+      <c r="K31">
+        <f>455-J31</f>
+        <v>11</v>
+      </c>
+      <c r="L31">
+        <v>75</v>
+      </c>
+      <c r="M31">
+        <v>280</v>
+      </c>
+      <c r="N31">
+        <f>455-M31</f>
+        <v>175</v>
+      </c>
+      <c r="O31">
+        <v>126</v>
+      </c>
+      <c r="P31">
+        <v>231</v>
+      </c>
+      <c r="Q31">
+        <f>455-P31</f>
+        <v>224</v>
+      </c>
+      <c r="R31">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>